<commit_message>
Sq. Class to Struct
</commit_message>
<xml_diff>
--- a/Assets/LEGAL_MOVE_STATS.xlsx
+++ b/Assets/LEGAL_MOVE_STATS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\flynn\OneDrive\Dokumentumok\Programming\Unity Projects\Chess Programming\Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18BDE878-DAB9-4E62-9393-48F5EC65FD44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BBC3469-4BFA-4E11-8DB6-6773F81FF0E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="3135" windowWidth="29040" windowHeight="15720" xr2:uid="{985101F8-B5F9-448A-B986-F404846CEA50}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Castling Fixed</t>
   </si>
@@ -60,6 +60,9 @@
   </si>
   <si>
     <t>Escape Routing Opt.</t>
+  </si>
+  <si>
+    <t>Sq Class to Struct</t>
   </si>
 </sst>
 </file>
@@ -302,9 +305,6 @@
     <xf numFmtId="43" fontId="0" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -327,6 +327,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="5" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -440,9 +443,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$C$1:$G$1</c:f>
+              <c:f>Sheet1!$C$1:$H$1</c:f>
               <c:strCache>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>Castling Fixed</c:v>
                 </c:pt>
@@ -458,15 +461,18 @@
                 <c:pt idx="4">
                   <c:v>Escape Routing Opt.</c:v>
                 </c:pt>
+                <c:pt idx="5">
+                  <c:v>Sq Class to Struct</c:v>
+                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$G$2</c:f>
+              <c:f>Sheet1!$C$2:$H$2</c:f>
               <c:numCache>
                 <c:formatCode>_-* #,##0_-;\-* #,##0_-;_-* "-"??_-;_-@_-</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -481,6 +487,9 @@
                 </c:pt>
                 <c:pt idx="4" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)">
                   <c:v>71280.802251092624</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)">
+                  <c:v>96950.950574367263</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1217,15 +1226,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>20835</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>196456</xdr:rowOff>
+      <xdr:colOff>14882</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>17859</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>1</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1315641</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>178594</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1570,11 +1579,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C8942EE-9018-4B14-A59B-6038BD1317B6}">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G10" sqref="G10"/>
+      <selection pane="bottomLeft" activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1586,10 +1595,11 @@
     <col min="5" max="5" width="22" style="2" customWidth="1"/>
     <col min="6" max="6" width="18.7109375" style="2" customWidth="1"/>
     <col min="7" max="7" width="19.85546875" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="2"/>
+    <col min="8" max="8" width="18.140625" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>4</v>
       </c>
@@ -1608,15 +1618,18 @@
       <c r="F1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="6" t="s">
         <v>7</v>
       </c>
+      <c r="H1" s="7" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="16" t="s">
+    <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="17"/>
+      <c r="B2" s="16"/>
       <c r="C2" s="9">
         <v>0</v>
       </c>
@@ -1632,172 +1645,196 @@
         <f>B8/F8</f>
         <v>57048.550071873506</v>
       </c>
-      <c r="G2" s="11">
+      <c r="G2" s="10">
         <f>B8/G8</f>
         <v>71280.802251092624</v>
       </c>
+      <c r="H2" s="19">
+        <f>B8/H8</f>
+        <v>96950.950574367263</v>
+      </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>1</v>
       </c>
       <c r="B3" s="8">
         <v>20</v>
       </c>
-      <c r="C3" s="18">
+      <c r="C3" s="17">
         <v>2E-3</v>
       </c>
-      <c r="D3" s="18">
+      <c r="D3" s="17">
         <v>0.01</v>
       </c>
-      <c r="E3" s="18">
+      <c r="E3" s="17">
         <v>0.01</v>
       </c>
-      <c r="F3" s="18">
+      <c r="F3" s="17">
         <v>0.01</v>
       </c>
-      <c r="G3" s="3">
+      <c r="G3" s="17">
         <v>8.9999999999999993E-3</v>
       </c>
+      <c r="H3" s="3">
+        <v>1E-3</v>
+      </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>2</v>
       </c>
       <c r="B4" s="8">
         <v>400</v>
       </c>
-      <c r="C4" s="18">
+      <c r="C4" s="17">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="D4" s="18">
+      <c r="D4" s="17">
         <v>4.2999999999999997E-2</v>
       </c>
-      <c r="E4" s="18">
+      <c r="E4" s="17">
         <v>4.2999999999999997E-2</v>
       </c>
-      <c r="F4" s="18">
+      <c r="F4" s="17">
         <v>0.01</v>
       </c>
-      <c r="G4" s="3">
+      <c r="G4" s="17">
         <v>8.9999999999999993E-3</v>
       </c>
+      <c r="H4" s="3">
+        <v>3.0000000000000001E-3</v>
+      </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>3</v>
       </c>
       <c r="B5" s="8">
         <v>8902</v>
       </c>
-      <c r="C5" s="19">
+      <c r="C5" s="18">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="D5" s="18">
+      <c r="D5" s="17">
         <v>1.2290000000000001</v>
       </c>
-      <c r="E5" s="18">
+      <c r="E5" s="17">
         <v>1.2290000000000001</v>
       </c>
-      <c r="F5" s="18">
+      <c r="F5" s="17">
         <v>0.11700000000000001</v>
       </c>
-      <c r="G5" s="3">
+      <c r="G5" s="17">
         <v>0.94</v>
       </c>
+      <c r="H5" s="3">
+        <v>7.0000000000000007E-2</v>
+      </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>4</v>
       </c>
       <c r="B6" s="8">
         <v>197281</v>
       </c>
-      <c r="C6" s="19">
+      <c r="C6" s="18">
         <v>0.66400000000000003</v>
       </c>
-      <c r="D6" s="18">
+      <c r="D6" s="17">
         <v>40.79</v>
       </c>
-      <c r="E6" s="18">
+      <c r="E6" s="17">
         <v>4.7939999999999996</v>
       </c>
-      <c r="F6" s="18">
+      <c r="F6" s="17">
         <v>3.5550000000000002</v>
       </c>
-      <c r="G6" s="3">
+      <c r="G6" s="17">
         <v>2.8620000000000001</v>
       </c>
+      <c r="H6" s="3">
+        <v>1.9590000000000001</v>
+      </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>5</v>
       </c>
       <c r="B7" s="8">
         <v>4865609</v>
       </c>
-      <c r="C7" s="19">
+      <c r="C7" s="18">
         <v>16.52</v>
       </c>
-      <c r="D7" s="19">
+      <c r="D7" s="18">
         <v>1010</v>
       </c>
-      <c r="E7" s="19">
+      <c r="E7" s="18">
         <v>101</v>
       </c>
-      <c r="F7" s="18">
+      <c r="F7" s="17">
         <v>84.33</v>
       </c>
-      <c r="G7" s="3">
+      <c r="G7" s="17">
         <v>67.363</v>
       </c>
+      <c r="H7" s="3">
+        <v>49.692999999999998</v>
+      </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>6</v>
       </c>
       <c r="B8" s="8">
         <v>119060324</v>
       </c>
-      <c r="C8" s="19">
+      <c r="C8" s="18">
         <v>363.8</v>
       </c>
-      <c r="D8" s="18"/>
-      <c r="E8" s="19">
+      <c r="D8" s="17"/>
+      <c r="E8" s="18">
         <v>1402</v>
       </c>
-      <c r="F8" s="18">
+      <c r="F8" s="17">
         <v>2087</v>
       </c>
-      <c r="G8" s="3">
+      <c r="G8" s="17">
         <v>1670.3</v>
       </c>
+      <c r="H8" s="3">
+        <v>1228.047</v>
+      </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>7</v>
       </c>
       <c r="B9" s="8">
         <v>3195901860</v>
       </c>
-      <c r="C9" s="18"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="3"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="3"/>
     </row>
-    <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="12">
+    <row r="10" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="11">
         <v>8</v>
       </c>
-      <c r="B10" s="13">
+      <c r="B10" s="12">
         <v>84998978956</v>
       </c>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="15"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Move Gen memory management
</commit_message>
<xml_diff>
--- a/Assets/LEGAL_MOVE_STATS.xlsx
+++ b/Assets/LEGAL_MOVE_STATS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\flynn\OneDrive\Dokumentumok\Programming\Unity Projects\Chess Programming\Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DBA0BF8-E571-49C8-9C16-5542BFFC7447}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A42AE8A-EA46-4114-AA3E-331ECD051B2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="3135" windowWidth="29040" windowHeight="15720" xr2:uid="{985101F8-B5F9-448A-B986-F404846CEA50}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Castling Fixed</t>
   </si>
@@ -72,6 +72,9 @@
   </si>
   <si>
     <t>Undo move opt.</t>
+  </si>
+  <si>
+    <t>Memory Man.</t>
   </si>
 </sst>
 </file>
@@ -146,7 +149,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -277,27 +280,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -350,25 +338,13 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -483,9 +459,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'MOVE GENERATION'!$C$1:$K$1</c:f>
+              <c:f>'MOVE GENERATION'!$C$1:$L$1</c:f>
               <c:strCache>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>Castling Fixed</c:v>
                 </c:pt>
@@ -512,16 +488,19 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>Undo move opt.</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Memory Man.</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'MOVE GENERATION'!$C$2:$K$2</c:f>
+              <c:f>'MOVE GENERATION'!$C$2:$L$2</c:f>
               <c:numCache>
                 <c:formatCode>_-* #,##0_-;\-* #,##0_-;_-* "-"??_-;_-@_-</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -548,6 +527,9 @@
                 </c:pt>
                 <c:pt idx="8" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)">
                   <c:v>263669.71615609311</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)">
+                  <c:v>310534.09319127299</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1637,11 +1619,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C8942EE-9018-4B14-A59B-6038BD1317B6}">
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K8" sqref="K8"/>
+      <selection pane="bottomLeft" activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1657,45 +1639,49 @@
     <col min="9" max="9" width="19.140625" style="2" customWidth="1"/>
     <col min="10" max="10" width="20.28515625" style="2" customWidth="1"/>
     <col min="11" max="11" width="21" style="2" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="2"/>
+    <col min="12" max="12" width="17.42578125" style="2" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="22" t="s">
+    <row r="1" spans="1:12" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="23" t="s">
+      <c r="C1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="23" t="s">
+      <c r="D1" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="23" t="s">
+      <c r="E1" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="23" t="s">
+      <c r="F1" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="23" t="s">
+      <c r="G1" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="H1" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="23" t="s">
+      <c r="I1" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="23" t="s">
+      <c r="J1" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="24" t="s">
+      <c r="K1" s="18" t="s">
         <v>11</v>
       </c>
+      <c r="L1" s="19" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="2" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
         <v>5</v>
       </c>
@@ -1731,47 +1717,54 @@
         <f>$B8/J8</f>
         <v>203025.98268503093</v>
       </c>
-      <c r="K2" s="13">
+      <c r="K2" s="14">
         <f>$B8/K8</f>
         <v>263669.71615609311</v>
       </c>
+      <c r="L2" s="13">
+        <f>$B8/L8</f>
+        <v>310534.09319127299</v>
+      </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
         <v>1</v>
       </c>
-      <c r="B3" s="18">
+      <c r="B3" s="6">
         <v>20</v>
       </c>
-      <c r="C3" s="19">
+      <c r="C3" s="17">
         <v>2E-3</v>
       </c>
-      <c r="D3" s="19">
+      <c r="D3" s="17">
         <v>0.01</v>
       </c>
-      <c r="E3" s="19">
+      <c r="E3" s="17">
         <v>0.01</v>
       </c>
-      <c r="F3" s="19">
+      <c r="F3" s="17">
         <v>0.01</v>
       </c>
-      <c r="G3" s="19">
+      <c r="G3" s="17">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="H3" s="19">
+      <c r="H3" s="17">
         <v>1E-3</v>
       </c>
-      <c r="I3" s="19">
+      <c r="I3" s="17">
         <v>1E-3</v>
       </c>
-      <c r="J3" s="19">
+      <c r="J3" s="17">
         <v>1E-3</v>
       </c>
-      <c r="K3" s="20">
+      <c r="K3" s="17">
         <v>1E-3</v>
       </c>
+      <c r="L3" s="3">
+        <v>1E-3</v>
+      </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>2</v>
       </c>
@@ -1802,18 +1795,21 @@
       <c r="J4" s="17">
         <v>1E-3</v>
       </c>
-      <c r="K4" s="3">
+      <c r="K4" s="17">
         <v>1E-3</v>
       </c>
+      <c r="L4" s="3">
+        <v>1E-3</v>
+      </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>3</v>
       </c>
       <c r="B5" s="6">
         <v>8902</v>
       </c>
-      <c r="C5" s="21">
+      <c r="C5" s="20">
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="D5" s="17">
@@ -1837,18 +1833,21 @@
       <c r="J5" s="17">
         <v>3.5000000000000003E-2</v>
       </c>
-      <c r="K5" s="3">
+      <c r="K5" s="17">
         <v>2.5000000000000001E-2</v>
       </c>
+      <c r="L5" s="3">
+        <v>1.6E-2</v>
+      </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>4</v>
       </c>
       <c r="B6" s="6">
         <v>197281</v>
       </c>
-      <c r="C6" s="21">
+      <c r="C6" s="20">
         <v>0.66400000000000003</v>
       </c>
       <c r="D6" s="17">
@@ -1872,24 +1871,27 @@
       <c r="J6" s="17">
         <v>0.97</v>
       </c>
-      <c r="K6" s="3">
+      <c r="K6" s="17">
         <v>0.69799999999999995</v>
       </c>
+      <c r="L6" s="3">
+        <v>0.48499999999999999</v>
+      </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>5</v>
       </c>
       <c r="B7" s="6">
         <v>4865609</v>
       </c>
-      <c r="C7" s="21">
+      <c r="C7" s="20">
         <v>16.52</v>
       </c>
-      <c r="D7" s="21">
+      <c r="D7" s="20">
         <v>1010</v>
       </c>
-      <c r="E7" s="21">
+      <c r="E7" s="20">
         <v>101</v>
       </c>
       <c r="F7" s="17">
@@ -1907,22 +1909,25 @@
       <c r="J7" s="17">
         <v>23.937000000000001</v>
       </c>
-      <c r="K7" s="3">
+      <c r="K7" s="17">
         <v>18.552</v>
       </c>
+      <c r="L7" s="3">
+        <v>15.571999999999999</v>
+      </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>6</v>
       </c>
       <c r="B8" s="6">
         <v>119060324</v>
       </c>
-      <c r="C8" s="21">
+      <c r="C8" s="20">
         <v>363.8</v>
       </c>
       <c r="D8" s="17"/>
-      <c r="E8" s="21">
+      <c r="E8" s="20">
         <v>1402</v>
       </c>
       <c r="F8" s="17">
@@ -1940,11 +1945,14 @@
       <c r="J8" s="17">
         <v>586.42899999999997</v>
       </c>
-      <c r="K8" s="3">
+      <c r="K8" s="17">
         <v>451.55099999999999</v>
       </c>
+      <c r="L8" s="3">
+        <v>383.40499999999997</v>
+      </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>7</v>
       </c>
@@ -1959,9 +1967,10 @@
       <c r="H9" s="17"/>
       <c r="I9" s="17"/>
       <c r="J9" s="17"/>
-      <c r="K9" s="3"/>
+      <c r="K9" s="17"/>
+      <c r="L9" s="3"/>
     </row>
-    <row r="10" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="9">
         <v>8</v>
       </c>
@@ -1976,7 +1985,8 @@
       <c r="H10" s="11"/>
       <c r="I10" s="11"/>
       <c r="J10" s="11"/>
-      <c r="K10" s="12"/>
+      <c r="K10" s="11"/>
+      <c r="L10" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>